<commit_message>
without working date inserting
</commit_message>
<xml_diff>
--- a/fun.xlsx
+++ b/fun.xlsx
@@ -14,12 +14,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
-  <si>
-    <t>цйа</t>
-  </si>
-  <si>
-    <t>іа</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+  <si>
+    <t xml:space="preserve">Иванов </t>
+  </si>
+  <si>
+    <t>Васильков</t>
+  </si>
+  <si>
+    <t>Петренко</t>
+  </si>
+  <si>
+    <t>Барахты</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Махно </t>
+  </si>
+  <si>
+    <t>Козятие</t>
+  </si>
+  <si>
+    <t>Степан</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Жорновка </t>
   </si>
 </sst>
 </file>
@@ -356,7 +374,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -372,6 +390,30 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>